<commit_message>
dodnie pliku w R
</commit_message>
<xml_diff>
--- a/dane.xlsx
+++ b/dane.xlsx
@@ -5,10 +5,10 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="F:\R\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="F:\PROJEKTY\Statystyka-w-R\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C6384E3F-4E39-4115-AE38-200BAD72DCC2}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{409C9343-CF40-443E-A055-FEE9BBEBD094}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -5115,7 +5115,7 @@
   <dimension ref="A1:F132"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E1" sqref="E1"/>
+      <selection activeCell="L19" sqref="L19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>